<commit_message>
Avanço més la pràctica Ia.
</commit_message>
<xml_diff>
--- a/graphs/practica_Ia/dades_estacionari.xlsx
+++ b/graphs/practica_Ia/dades_estacionari.xlsx
@@ -8,20 +8,53 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Miguel\UAB\TERCER\LAB Termo\Repositori\graphs\practica_Ia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BFBDA9-75FD-4BA7-AB30-EDB9EC016FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63465AA-D7B7-45CB-9D0B-07807928E2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1512" yWindow="1092" windowWidth="21624" windowHeight="11244" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-870" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -228,6 +261,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Hoja1!$B$13:$M$13</c:f>
@@ -353,6 +400,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Hoja1!$B$13:$M$13</c:f>
@@ -478,6 +539,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Hoja1!$B$13:$M$13</c:f>
@@ -1323,15 +1398,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>243840</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>82867</xdr:rowOff>
+      <xdr:rowOff>88582</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>88582</xdr:rowOff>
+      <xdr:colOff>303451</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>118008</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1622,10 +1697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1912,6 +1987,47 @@
         <v>9</v>
       </c>
     </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" cm="1">
+        <f t="array" ref="B17:C21">LOGEST(B12:M12,B13:M13,TRUE,TRUE)</f>
+        <v>0.98897062045643169</v>
+      </c>
+      <c r="C17">
+        <v>63.636069650438408</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>2.4501709526838699E-3</v>
+      </c>
+      <c r="C18">
+        <v>0.15910397216055885</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>0.67201325595693795</v>
+      </c>
+      <c r="C19">
+        <v>0.29299783117366879</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>20.489037077324927</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>1.7589373039700587</v>
+      </c>
+      <c r="C21">
+        <v>0.85847729072473711</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Practica Ia: abstract, resultats i conclusions acabats.
</commit_message>
<xml_diff>
--- a/graphs/practica_Ia/dades_estacionari.xlsx
+++ b/graphs/practica_Ia/dades_estacionari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Miguel\UAB\TERCER\LAB Termo\Repositori\graphs\practica_Ia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BE38FE-25AA-4625-B7B7-B5F0ED8C53B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADE0F25-4B48-411F-AF80-84B9CD4E6040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,6 +123,3064 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Alumini</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.28572115058901748"/>
+                  <c:y val="-0.60071636190104338"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>29.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>63.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>77.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>119</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6632-4612-8494-FC8D954DC23F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1963008672"/>
+        <c:axId val="1963009152"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1963008672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1963009152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1963009152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1963008672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Llauto</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.9599737532808399E-2"/>
+                  <c:y val="-0.6649442257217848"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>26.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>72.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>108.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D80A-4F13-9200-F8C52FBB721F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1954039360"/>
+        <c:axId val="1954033600"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1954039360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1954033600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1954033600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1954039360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.0044181977252842E-2"/>
+                  <c:y val="-0.70565033537474486"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>24.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8D23-4168-AD5A-AE0AF2468F92}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1891781392"/>
+        <c:axId val="1962705488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1891781392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1962705488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1962705488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1891781392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>420444</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AD7EB61-C3DC-DAB2-D882-7E478F8254E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB15B75D-7E44-F93C-8794-8A29D091C080}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>493058</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>10757</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F4FF68B-AD48-271A-500D-6AB958B5CFF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,8 +3448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,9 +3586,18 @@
         <v>25.8</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="F5" s="2">
+        <f>AVERAGE(F2:F4)/2</f>
+        <v>1.5241666666666667</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:H5" si="0">AVERAGE(G2:G4)/2</f>
+        <v>1.5183333333333333</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5733333333333333</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -747,7 +3814,10 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3">
+        <f>SQRT(0.1^2+_xlfn.STDEV.S(E2:E4)^2)</f>
+        <v>0.18257418583505428</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1444,5 +4514,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>